<commit_message>
translated all sentences into korean
</commit_message>
<xml_diff>
--- a/experiments/1-baseline/english-sentences.xlsx
+++ b/experiments/1-baseline/english-sentences.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/git/korean-scope/experiments/1-baseline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/1-baseline/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7DE1EF2C-B221-F74D-8ECD-9484A9A04DC0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="6680" windowWidth="25320" windowHeight="14380" tabRatio="500"/>
+    <workbookView xWindow="5320" yWindow="460" windowWidth="25320" windowHeight="14380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">sentence </t>
   </si>
@@ -81,13 +82,115 @@
   </si>
   <si>
     <t>A girl pet every dog</t>
+  </si>
+  <si>
+    <t>korean</t>
+  </si>
+  <si>
+    <t>모든 해적이 통애 기대어 있다</t>
+  </si>
+  <si>
+    <t>통에 기대어 있다</t>
+  </si>
+  <si>
+    <t>해적이 모든 통에 기대어 있다</t>
+  </si>
+  <si>
+    <t>모든 해적이 물고기를 잡았다</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 해적 한사람이 모든 통에 기대어 있다</t>
+  </si>
+  <si>
+    <t>해적 한사람이 모든 물고기를 잡았다</t>
+  </si>
+  <si>
+    <t>모든 해적이 통 하나에 기대어 있다</t>
+  </si>
+  <si>
+    <t>모든 해적이 낚시대 하나를 잡고 있다</t>
+  </si>
+  <si>
+    <t>해적 한사람이 모든 낚시대를 잡고 있다</t>
+  </si>
+  <si>
+    <t>해적 한사람이 모든 상어를 먹이고 있다</t>
+  </si>
+  <si>
+    <t>모든 해적이 병 하나를 잡고 있다</t>
+  </si>
+  <si>
+    <t>해적 한사람이 모든 병을 잡고 있다</t>
+  </si>
+  <si>
+    <t>모든 상어가 물고기 한마리를 물고 있다</t>
+  </si>
+  <si>
+    <t>상어 한마리가 모든 물고기를 물고 있다</t>
+  </si>
+  <si>
+    <t>모든 상어가 해적 한사람을 공격했다</t>
+  </si>
+  <si>
+    <t>상어 한마리가 모든 해적을 공격했다</t>
+  </si>
+  <si>
+    <t>모든 여자아이가 강아지 한마리를 쓰다듬고 있다</t>
+  </si>
+  <si>
+    <t>여자아이 하나가 모든 강아지를 쓰다듬었다</t>
+  </si>
+  <si>
+    <t xml:space="preserve">모든 해적이 물고기 한마리를 잡았다 </t>
+  </si>
+  <si>
+    <t>해적이 모든 물고기를 잡았다</t>
+  </si>
+  <si>
+    <t>모든 해적이 낚시대를 잡고 있다</t>
+  </si>
+  <si>
+    <t>해적이 모든 낚시대를 잡고 있다</t>
+  </si>
+  <si>
+    <t>모든 해적이 상어를 먹였다</t>
+  </si>
+  <si>
+    <t>모든 해적이 상어 한마리를 먹였다</t>
+  </si>
+  <si>
+    <t>해적이 모든 상어를 먹였다</t>
+  </si>
+  <si>
+    <t>모든 해적이 병을 잡고 있다</t>
+  </si>
+  <si>
+    <t>해적이 모든 병을 잡고 있다</t>
+  </si>
+  <si>
+    <t>모든 상어가 물고기를 물고있다</t>
+  </si>
+  <si>
+    <t>상어가 모든 물고기를 물고 있다</t>
+  </si>
+  <si>
+    <t>모든 상어가 해적을 공격했다</t>
+  </si>
+  <si>
+    <t>상어가 모든 해적을 공격했다</t>
+  </si>
+  <si>
+    <t>모든 여자아이가 강아지를 쓰다듬고 있다</t>
+  </si>
+  <si>
+    <t>여자아이가 모든 강아지를 쓰다듬었다</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,15 +207,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="CharisSIL"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="CharisSIL"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,11 +244,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,152 +529,291 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2">
+      <c r="C1" s="4"/>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3">
+      <c r="C2" s="4"/>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4">
+      <c r="C3" s="4"/>
+      <c r="D3" s="2"/>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="C4" s="4"/>
+      <c r="D4" s="2"/>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6">
+      <c r="C5" s="4"/>
+      <c r="D5" s="2"/>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="C6" s="4"/>
+      <c r="D6" s="2"/>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A8">
+      <c r="C7" s="4"/>
+      <c r="D7" s="2"/>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="C8" s="4"/>
+      <c r="D8" s="2"/>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A10">
+      <c r="C9" s="4"/>
+      <c r="D9" s="2"/>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4">
         <v>5</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="C10" s="4"/>
+      <c r="D10" s="2"/>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A12">
+      <c r="C11" s="4"/>
+      <c r="D11" s="2"/>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4">
         <v>6</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="C12" s="4"/>
+      <c r="D12" s="2"/>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4">
         <v>6</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A14">
+      <c r="C13" s="4"/>
+      <c r="D13" s="2"/>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4">
         <v>7</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="C14" s="4"/>
+      <c r="D14" s="2"/>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4">
         <v>7</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16">
+      <c r="C15" s="4"/>
+      <c r="D15" s="2"/>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="4">
         <v>8</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="C16" s="4"/>
+      <c r="D16" s="2"/>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="4">
         <v>8</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="2"/>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added scrambled options to translations
</commit_message>
<xml_diff>
--- a/experiments/1-baseline/english-sentences.xlsx
+++ b/experiments/1-baseline/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/1-baseline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7DE1EF2C-B221-F74D-8ECD-9484A9A04DC0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{59DA82B5-5AA1-DD43-91ED-B86264FA1718}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="460" windowWidth="25320" windowHeight="14380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="1340" windowWidth="32660" windowHeight="19120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t xml:space="preserve">sentence </t>
   </si>
@@ -184,6 +184,102 @@
   </si>
   <si>
     <t>여자아이가 모든 강아지를 쓰다듬었다</t>
+  </si>
+  <si>
+    <t>통에 모든 해적이 기대어 있다</t>
+  </si>
+  <si>
+    <t>통 하나에 모든 해적이 기대어 있다</t>
+  </si>
+  <si>
+    <t>모든 통에 해적 한사람이 기대어 있다</t>
+  </si>
+  <si>
+    <t>모든 통에 해적이 기대어 있다</t>
+  </si>
+  <si>
+    <t>물고기 한마리를 해적 한사람이 잡았다</t>
+  </si>
+  <si>
+    <t>물고기를 모든 해적이 잡았다</t>
+  </si>
+  <si>
+    <t>모든 물고기를 해적 한사람이 잡았다</t>
+  </si>
+  <si>
+    <t>모든 물고기를 해적이 잡았다</t>
+  </si>
+  <si>
+    <t>낚시대 하나를 모든 해적이 잡고 있다</t>
+  </si>
+  <si>
+    <t>낚시대를 모든 해적이 잡고 있다</t>
+  </si>
+  <si>
+    <t>모든 낚시대를 해적 한사람이 잡고 있다</t>
+  </si>
+  <si>
+    <t>모든 낚시대를 해적이 잡고 있다</t>
+  </si>
+  <si>
+    <t>상어 한마리를 모든 해적이 먹였다</t>
+  </si>
+  <si>
+    <t>상어를 모든 해적이 먹였다</t>
+  </si>
+  <si>
+    <t>모든 상어를 해적 한사람이 먹였다</t>
+  </si>
+  <si>
+    <t>모든 상어를 해적이 먹였다</t>
+  </si>
+  <si>
+    <t>병 하나를 모든 해적이 잡고 있다</t>
+  </si>
+  <si>
+    <t>병을 모든 해적이 잡고 있다</t>
+  </si>
+  <si>
+    <t>모든 병을 해적 한사람이 잡고 있다</t>
+  </si>
+  <si>
+    <t>모든 병을 해적이 잡고 있다</t>
+  </si>
+  <si>
+    <t>물고기 한마리를 모든 상어가 물고 있다</t>
+  </si>
+  <si>
+    <t>물고기를 모든 상어가 물고 있다</t>
+  </si>
+  <si>
+    <t>모든 물고기를 상어 한마리가 물고 있다</t>
+  </si>
+  <si>
+    <t>모든 물고기를 상어가 물고 있다</t>
+  </si>
+  <si>
+    <t>해적 한사람을 모든 상어가 공격했다</t>
+  </si>
+  <si>
+    <t>해적을 모든 상어가 공격했다</t>
+  </si>
+  <si>
+    <t>모든 해적을 상어 한마리가 공격했다</t>
+  </si>
+  <si>
+    <t>모든 해적을 상어가 공격했다</t>
+  </si>
+  <si>
+    <t>강아지 한마리를 모든 여자아이가 쓰다듬고 있다</t>
+  </si>
+  <si>
+    <t>강아지를 모든 여자아이가 쓰다듬고 있다</t>
+  </si>
+  <si>
+    <t>모든 강아지를 여자아이 하나가 쓰다듬고 있었다</t>
+  </si>
+  <si>
+    <t>모든 강아지를 여자아이가 쓰다듬고 있었다</t>
   </si>
 </sst>
 </file>
@@ -530,18 +626,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:16">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -553,7 +649,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:16">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -571,8 +667,14 @@
       <c r="H2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="L2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -587,8 +689,14 @@
       <c r="H3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="L3" t="s">
+        <v>54</v>
+      </c>
+      <c r="P3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -603,8 +711,14 @@
       <c r="H4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="L4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -619,8 +733,14 @@
       <c r="H5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="L5" t="s">
+        <v>58</v>
+      </c>
+      <c r="P5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -635,8 +755,14 @@
       <c r="H6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="L6" t="s">
+        <v>60</v>
+      </c>
+      <c r="P6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -651,8 +777,14 @@
       <c r="H7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+      <c r="P7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -667,8 +799,14 @@
       <c r="H8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="L8" t="s">
+        <v>64</v>
+      </c>
+      <c r="P8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="4">
         <v>4</v>
       </c>
@@ -683,8 +821,14 @@
       <c r="H9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="L9" t="s">
+        <v>66</v>
+      </c>
+      <c r="P9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="4">
         <v>5</v>
       </c>
@@ -699,8 +843,14 @@
       <c r="H10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="L10" t="s">
+        <v>68</v>
+      </c>
+      <c r="P10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -715,8 +865,14 @@
       <c r="H11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="L11" t="s">
+        <v>70</v>
+      </c>
+      <c r="P11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -731,8 +887,14 @@
       <c r="H12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="L12" t="s">
+        <v>72</v>
+      </c>
+      <c r="P12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="4">
         <v>6</v>
       </c>
@@ -747,8 +909,14 @@
       <c r="H13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="L13" t="s">
+        <v>74</v>
+      </c>
+      <c r="P13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="4">
         <v>7</v>
       </c>
@@ -763,8 +931,14 @@
       <c r="H14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="L14" t="s">
+        <v>76</v>
+      </c>
+      <c r="P14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="4">
         <v>7</v>
       </c>
@@ -779,8 +953,14 @@
       <c r="H15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="L15" t="s">
+        <v>78</v>
+      </c>
+      <c r="P15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="4">
         <v>8</v>
       </c>
@@ -795,8 +975,14 @@
       <c r="H16" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="L16" t="s">
+        <v>80</v>
+      </c>
+      <c r="P16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="4">
         <v>8</v>
       </c>
@@ -810,6 +996,12 @@
       </c>
       <c r="H17" t="s">
         <v>51</v>
+      </c>
+      <c r="L17" t="s">
+        <v>82</v>
+      </c>
+      <c r="P17" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created new folder under views (views_korean) and duplicated all files of questionnaires
</commit_message>
<xml_diff>
--- a/experiments/1-baseline/english-sentences.xlsx
+++ b/experiments/1-baseline/english-sentences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/1-baseline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{59DA82B5-5AA1-DD43-91ED-B86264FA1718}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BDA74928-214C-6149-BCA0-44EE7D7460DA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="1340" windowWidth="32660" windowHeight="19120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,7 +99,7 @@
     <t>모든 해적이 물고기를 잡았다</t>
   </si>
   <si>
-    <t xml:space="preserve"> 해적 한사람이 모든 통에 기대어 있다</t>
+    <t>해적 한사람이 모든 통에 기대어 있다</t>
   </si>
   <si>
     <t>해적 한사람이 모든 물고기를 잡았다</t>
@@ -628,13 +628,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="7" max="7" width="27.1640625" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">

</xml_diff>

<commit_message>
highlighted sentences to be recorded
yellow highlight = default translation
orange highlight = scrambled option
</commit_message>
<xml_diff>
--- a/experiments/1-baseline/english-sentences.xlsx
+++ b/experiments/1-baseline/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/1-baseline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BDA74928-214C-6149-BCA0-44EE7D7460DA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3C504DB9-5A4A-9F4D-B654-EC5F88476360}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="1340" windowWidth="32660" windowHeight="19120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2900" yWindow="460" windowWidth="32660" windowHeight="19120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t xml:space="preserve">sentence </t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>모든 해적이 통애 기대어 있다</t>
-  </si>
-  <si>
-    <t>통에 기대어 있다</t>
   </si>
   <si>
     <t>해적이 모든 통에 기대어 있다</t>
@@ -320,12 +317,24 @@
       <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -340,12 +349,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,7 +640,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -659,20 +670,22 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="2"/>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="L2" s="5" t="s">
         <v>52</v>
       </c>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
       <c r="P2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -684,17 +697,22 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="2"/>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
+      <c r="E3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" t="s">
         <v>54</v>
-      </c>
-      <c r="P3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -706,17 +724,22 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="2"/>
-      <c r="E4" t="s">
-        <v>37</v>
-      </c>
+      <c r="E4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
       <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" t="s">
         <v>56</v>
-      </c>
-      <c r="P4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -728,17 +751,22 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
+      <c r="E5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
       <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" t="s">
         <v>58</v>
-      </c>
-      <c r="P5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -750,17 +778,22 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="2"/>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
+      <c r="E6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
       <c r="H6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" t="s">
         <v>60</v>
-      </c>
-      <c r="P6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -772,17 +805,22 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="2"/>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
+      <c r="E7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
       <c r="H7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" t="s">
         <v>62</v>
-      </c>
-      <c r="P7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -794,17 +832,22 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="2"/>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
+      <c r="E8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
       <c r="H8" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" t="s">
         <v>64</v>
-      </c>
-      <c r="P8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -816,17 +859,22 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="2"/>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
+      <c r="E9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
       <c r="H9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" t="s">
         <v>66</v>
-      </c>
-      <c r="P9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -838,17 +886,22 @@
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="2"/>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
+      <c r="E10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
       <c r="H10" t="s">
-        <v>44</v>
-      </c>
-      <c r="L10" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" t="s">
         <v>68</v>
-      </c>
-      <c r="P10" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -860,17 +913,22 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2"/>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
+      <c r="E11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
       <c r="H11" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" t="s">
         <v>70</v>
-      </c>
-      <c r="P11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -882,17 +940,22 @@
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
+      <c r="E12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
       <c r="H12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" t="s">
         <v>72</v>
-      </c>
-      <c r="P12" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -904,17 +967,22 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="2"/>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
+      <c r="E13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
       <c r="H13" t="s">
-        <v>47</v>
-      </c>
-      <c r="L13" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" t="s">
         <v>74</v>
-      </c>
-      <c r="P13" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -926,17 +994,22 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
-      <c r="E14" t="s">
-        <v>33</v>
-      </c>
+      <c r="E14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
       <c r="H14" t="s">
-        <v>48</v>
-      </c>
-      <c r="L14" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" t="s">
         <v>76</v>
-      </c>
-      <c r="P14" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -948,17 +1021,22 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2"/>
-      <c r="E15" t="s">
-        <v>34</v>
-      </c>
+      <c r="E15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
       <c r="H15" t="s">
-        <v>49</v>
-      </c>
-      <c r="L15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" t="s">
         <v>78</v>
-      </c>
-      <c r="P15" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -970,17 +1048,22 @@
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="2"/>
-      <c r="E16" t="s">
-        <v>35</v>
-      </c>
+      <c r="E16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
       <c r="H16" t="s">
-        <v>50</v>
-      </c>
-      <c r="L16" t="s">
+        <v>49</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" t="s">
         <v>80</v>
-      </c>
-      <c r="P16" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -992,17 +1075,22 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2"/>
-      <c r="E17" t="s">
-        <v>36</v>
-      </c>
+      <c r="E17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
       <c r="H17" t="s">
-        <v>51</v>
-      </c>
-      <c r="L17" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" t="s">
         <v>82</v>
-      </c>
-      <c r="P17" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
numbered sentences to organized recorded files, also revised some sentences
</commit_message>
<xml_diff>
--- a/experiments/1-baseline/english-sentences.xlsx
+++ b/experiments/1-baseline/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/1-baseline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{46F57CCB-6EEB-DE47-AA79-6AE107677E1C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9DB4CC73-85BF-044D-B723-20A5311526E0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="460" windowWidth="32660" windowHeight="19120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="27300" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,51 +96,6 @@
     <t>모든 해적이 물고기를 잡았다</t>
   </si>
   <si>
-    <t>해적 한사람이 모든 통에 기대어 있다</t>
-  </si>
-  <si>
-    <t>해적 한사람이 모든 물고기를 잡았다</t>
-  </si>
-  <si>
-    <t>모든 해적이 통 하나에 기대어 있다</t>
-  </si>
-  <si>
-    <t>모든 해적이 낚시대 하나를 잡고 있다</t>
-  </si>
-  <si>
-    <t>해적 한사람이 모든 낚시대를 잡고 있다</t>
-  </si>
-  <si>
-    <t>해적 한사람이 모든 상어를 먹이고 있다</t>
-  </si>
-  <si>
-    <t>모든 해적이 병 하나를 잡고 있다</t>
-  </si>
-  <si>
-    <t>해적 한사람이 모든 병을 잡고 있다</t>
-  </si>
-  <si>
-    <t>모든 상어가 물고기 한마리를 물고 있다</t>
-  </si>
-  <si>
-    <t>상어 한마리가 모든 물고기를 물고 있다</t>
-  </si>
-  <si>
-    <t>모든 상어가 해적 한사람을 공격했다</t>
-  </si>
-  <si>
-    <t>상어 한마리가 모든 해적을 공격했다</t>
-  </si>
-  <si>
-    <t>모든 여자아이가 강아지 한마리를 쓰다듬고 있다</t>
-  </si>
-  <si>
-    <t>여자아이 하나가 모든 강아지를 쓰다듬었다</t>
-  </si>
-  <si>
-    <t xml:space="preserve">모든 해적이 물고기 한마리를 잡았다 </t>
-  </si>
-  <si>
     <t>해적이 모든 물고기를 잡았다</t>
   </si>
   <si>
@@ -153,9 +108,6 @@
     <t>모든 해적이 상어를 먹였다</t>
   </si>
   <si>
-    <t>모든 해적이 상어 한마리를 먹였다</t>
-  </si>
-  <si>
     <t>해적이 모든 상어를 먹였다</t>
   </si>
   <si>
@@ -186,97 +138,145 @@
     <t>통에 모든 해적이 기대어 있다</t>
   </si>
   <si>
-    <t>통 하나에 모든 해적이 기대어 있다</t>
-  </si>
-  <si>
-    <t>모든 통에 해적 한사람이 기대어 있다</t>
-  </si>
-  <si>
     <t>모든 통에 해적이 기대어 있다</t>
   </si>
   <si>
-    <t>물고기 한마리를 해적 한사람이 잡았다</t>
-  </si>
-  <si>
     <t>물고기를 모든 해적이 잡았다</t>
   </si>
   <si>
-    <t>모든 물고기를 해적 한사람이 잡았다</t>
-  </si>
-  <si>
     <t>모든 물고기를 해적이 잡았다</t>
   </si>
   <si>
-    <t>낚시대 하나를 모든 해적이 잡고 있다</t>
-  </si>
-  <si>
     <t>낚시대를 모든 해적이 잡고 있다</t>
   </si>
   <si>
-    <t>모든 낚시대를 해적 한사람이 잡고 있다</t>
-  </si>
-  <si>
     <t>모든 낚시대를 해적이 잡고 있다</t>
   </si>
   <si>
-    <t>상어 한마리를 모든 해적이 먹였다</t>
-  </si>
-  <si>
     <t>상어를 모든 해적이 먹였다</t>
   </si>
   <si>
-    <t>모든 상어를 해적 한사람이 먹였다</t>
-  </si>
-  <si>
     <t>모든 상어를 해적이 먹였다</t>
   </si>
   <si>
-    <t>병 하나를 모든 해적이 잡고 있다</t>
-  </si>
-  <si>
     <t>병을 모든 해적이 잡고 있다</t>
   </si>
   <si>
-    <t>모든 병을 해적 한사람이 잡고 있다</t>
-  </si>
-  <si>
     <t>모든 병을 해적이 잡고 있다</t>
   </si>
   <si>
-    <t>물고기 한마리를 모든 상어가 물고 있다</t>
-  </si>
-  <si>
     <t>물고기를 모든 상어가 물고 있다</t>
   </si>
   <si>
-    <t>모든 물고기를 상어 한마리가 물고 있다</t>
-  </si>
-  <si>
     <t>모든 물고기를 상어가 물고 있다</t>
   </si>
   <si>
-    <t>해적 한사람을 모든 상어가 공격했다</t>
-  </si>
-  <si>
     <t>해적을 모든 상어가 공격했다</t>
   </si>
   <si>
-    <t>모든 해적을 상어 한마리가 공격했다</t>
-  </si>
-  <si>
     <t>모든 해적을 상어가 공격했다</t>
   </si>
   <si>
-    <t>강아지 한마리를 모든 여자아이가 쓰다듬고 있다</t>
-  </si>
-  <si>
     <t>강아지를 모든 여자아이가 쓰다듬고 있다</t>
   </si>
   <si>
-    <t>모든 강아지를 여자아이 하나가 쓰다듬고 있었다</t>
-  </si>
-  <si>
     <t>모든 강아지를 여자아이가 쓰다듬고 있었다</t>
+  </si>
+  <si>
+    <t>1 모든 해적이 통 하나에 기대어 있다</t>
+  </si>
+  <si>
+    <t>1.1 통 하나에 모든 해적이 기대어 있다</t>
+  </si>
+  <si>
+    <t>2.1 모든 통에 해적 한사람이 기대어 있다</t>
+  </si>
+  <si>
+    <t>2 해적 한사람이 모든 통에 기대어 있다</t>
+  </si>
+  <si>
+    <t>3.1 물고기 한마리를 해적 한사람이 잡았다</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 모든 해적이 물고기 한마리를 잡았다 </t>
+  </si>
+  <si>
+    <t>4 해적 한사람이 모든 물고기를 잡았다</t>
+  </si>
+  <si>
+    <t>4.1 모든 물고기를 해적 한사람이 잡았다</t>
+  </si>
+  <si>
+    <t>5 모든 해적이 낚시대 하나를 잡고 있다</t>
+  </si>
+  <si>
+    <t>6 해적 한사람이 모든 낚시대를 잡고 있다</t>
+  </si>
+  <si>
+    <t>7 모든 해적이 상어 한마리를 먹였다</t>
+  </si>
+  <si>
+    <t>9 모든 해적이 병 하나를 잡고 있다</t>
+  </si>
+  <si>
+    <t>10 해적 한사람이 모든 병을 잡고 있다</t>
+  </si>
+  <si>
+    <t>11 모든 상어가 물고기 한마리를 물고 있다</t>
+  </si>
+  <si>
+    <t>12 상어 한마리가 모든 물고기를 물고 있다</t>
+  </si>
+  <si>
+    <t>13 모든 상어가 해적 한사람을 공격했다</t>
+  </si>
+  <si>
+    <t>14 상어 한마리가 모든 해적을 공격했다</t>
+  </si>
+  <si>
+    <t>15 모든 여자아이가 강아지 한마리를 쓰다듬고 있다</t>
+  </si>
+  <si>
+    <t>16 여자아이 하나가 모든 강아지를 쓰다듬었다</t>
+  </si>
+  <si>
+    <t>5.1 낚시대 하나를 모든 해적이 잡고 있다</t>
+  </si>
+  <si>
+    <t>6.1 모든 낚시대를 해적 한사람이 잡고 있다</t>
+  </si>
+  <si>
+    <t>7.1 상어 한마리를 모든 해적이 먹였다</t>
+  </si>
+  <si>
+    <t>8.1 모든 상어를 해적 한사람이 먹였다</t>
+  </si>
+  <si>
+    <t>9.1 병 하나를 모든 해적이 잡고 있다</t>
+  </si>
+  <si>
+    <t>10.1 모든 병을 해적 한사람이 잡고 있다</t>
+  </si>
+  <si>
+    <t>11.1 물고기 한마리를 모든 상어가 물고 있다</t>
+  </si>
+  <si>
+    <t>12.1 모든 물고기를 상어 한마리가 물고 있다</t>
+  </si>
+  <si>
+    <t>13.1 해적 한사람을 모든 상어가 공격했다</t>
+  </si>
+  <si>
+    <t>14.1 모든 해적을 상어 한마리가 공격했다</t>
+  </si>
+  <si>
+    <t>15.1 강아지 한마리를 모든 여자아이가 쓰다듬고 있다</t>
+  </si>
+  <si>
+    <t>8 해적 한사람이 모든 상어를 먹였다</t>
+  </si>
+  <si>
+    <t>16.1 모든 강아지를 여자아이 하나가 쓰다듬었다</t>
   </si>
 </sst>
 </file>
@@ -640,13 +640,13 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="7" max="7" width="27.1640625" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -671,7 +671,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="2"/>
       <c r="E2" s="6" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -685,7 +685,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -698,7 +698,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="2"/>
       <c r="E3" s="6" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -712,7 +712,7 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -725,7 +725,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="2"/>
       <c r="E4" s="6" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -739,7 +739,7 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -752,21 +752,21 @@
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="E5" s="6" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -779,21 +779,21 @@
       <c r="C6" s="4"/>
       <c r="D6" s="2"/>
       <c r="E6" s="6" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -806,21 +806,21 @@
       <c r="C7" s="4"/>
       <c r="D7" s="2"/>
       <c r="E7" s="6" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -833,21 +833,21 @@
       <c r="C8" s="4"/>
       <c r="D8" s="2"/>
       <c r="E8" s="6" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -860,21 +860,21 @@
       <c r="C9" s="4"/>
       <c r="D9" s="2"/>
       <c r="E9" s="6" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -887,21 +887,21 @@
       <c r="C10" s="4"/>
       <c r="D10" s="2"/>
       <c r="E10" s="6" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -914,21 +914,21 @@
       <c r="C11" s="4"/>
       <c r="D11" s="2"/>
       <c r="E11" s="6" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -941,21 +941,21 @@
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
       <c r="E12" s="6" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -968,21 +968,21 @@
       <c r="C13" s="4"/>
       <c r="D13" s="2"/>
       <c r="E13" s="6" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -995,21 +995,21 @@
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
       <c r="E14" s="6" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1022,21 +1022,21 @@
       <c r="C15" s="4"/>
       <c r="D15" s="2"/>
       <c r="E15" s="6" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1049,21 +1049,21 @@
       <c r="C16" s="4"/>
       <c r="D16" s="2"/>
       <c r="E16" s="6" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1076,21 +1076,21 @@
       <c r="C17" s="4"/>
       <c r="D17" s="2"/>
       <c r="E17" s="6" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
named the files using: [number]-[item type]-[aevery/everya]-[default/scrambled].m4a
</commit_message>
<xml_diff>
--- a/experiments/1-baseline/english-sentences.xlsx
+++ b/experiments/1-baseline/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/1-baseline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9DB4CC73-85BF-044D-B723-20A5311526E0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{14BBDFB2-5CB3-EF4F-9D2D-BD0292D1D41F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="27300" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16120" yWindow="460" windowWidth="17740" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>